<commit_message>
Fix figure of charset
</commit_message>
<xml_diff>
--- a/application_framework/application_framework/setting_guide/CustomizingConfigurations/charset.xlsx
+++ b/application_framework/application_framework/setting_guide/CustomizingConfigurations/charset.xlsx
@@ -163,7 +163,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -258,13 +258,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -299,6 +343,21 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -605,7 +664,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
@@ -832,7 +891,7 @@
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="13" t="s">
         <v>21</v>
       </c>
       <c r="F22" s="2"/>
@@ -840,11 +899,11 @@
     <row r="23" spans="1:6" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A23" s="2"/>
       <c r="B23" s="6"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="10" t="s">
+      <c r="C23" s="12"/>
+      <c r="D23" s="9" t="s">
         <v>0</v>
       </c>
+      <c r="E23" s="16"/>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" ht="16.5" x14ac:dyDescent="0.15">
@@ -853,8 +912,8 @@
       <c r="C24" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="8"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="15"/>
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6" ht="16.5" x14ac:dyDescent="0.15">

</xml_diff>